<commit_message>
Selenium Framework with TestNG & Logs generation
</commit_message>
<xml_diff>
--- a/TestSuite.xlsx
+++ b/TestSuite.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E71860-EA67-4C3F-B742-AB5143F4CAFD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453753DB-2B9C-4FFC-834C-EDA54E6D0615}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Run_Flag</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>TC_01</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -380,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,19 +407,11 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>